<commit_message>
Update Feb 5, 2020/
</commit_message>
<xml_diff>
--- a/wrangle/data/interventions/place-types-concordance.xlsx
+++ b/wrangle/data/interventions/place-types-concordance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/Dec-Update/wrangle/data/interventions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/CovidTimeline/wrangle/data/interventions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E9D137-7390-5C4E-B7F2-F5A452F47110}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBE6208-0974-6542-8FE9-D7DF418840CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25960" windowHeight="11320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25960" windowHeight="11320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAICS" sheetId="1" r:id="rId1"/>
@@ -18,21 +18,28 @@
     <sheet name="google" sheetId="3" r:id="rId3"/>
     <sheet name="industries-dict" sheetId="4" r:id="rId4"/>
     <sheet name="popctrs-dict" sheetId="5" r:id="rId5"/>
+    <sheet name="gtrends-dict" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NAICS!$A$1:$E$45</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="204">
   <si>
     <t>description</t>
   </si>
@@ -578,13 +585,79 @@
   </si>
   <si>
     <t>retail, non-essential retail, non-essential businesses, shopping malls, shopping centres</t>
+  </si>
+  <si>
+    <t>googletrends_cat</t>
+  </si>
+  <si>
+    <t>googletrends_id</t>
+  </si>
+  <si>
+    <t>Clubs &amp; Nightlife</t>
+  </si>
+  <si>
+    <t>Arts &amp; Entertainment</t>
+  </si>
+  <si>
+    <t>Beauty &amp; Fitness</t>
+  </si>
+  <si>
+    <t>Small Business</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Restaurants</t>
+  </si>
+  <si>
+    <t>Grocery &amp; Food Retailers</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Hobbies &amp; Leisure</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Bankruptcy</t>
+  </si>
+  <si>
+    <t>Business &amp; Corporate Law</t>
+  </si>
+  <si>
+    <t>Social Services</t>
+  </si>
+  <si>
+    <t>Business News</t>
+  </si>
+  <si>
+    <t>Housing &amp; Development</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Apparel</t>
+  </si>
+  <si>
+    <t>Home &amp; Garden</t>
+  </si>
+  <si>
+    <t>Alcoholic Beverages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +675,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -624,11 +705,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -638,8 +720,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{C29A9F8B-611F-4B4E-9EAD-C92FBB249969}"/>
   </cellStyles>
@@ -2400,8 +2484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000C3A94-B457-054D-BEB3-4CEBD1D7B7BF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2769,4 +2853,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A589B64-3508-C44C-B4D4-EFDF33F16175}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="gt_cat" xr:uid="{8D753641-4BD5-F543-B051-FB8C4BB46780}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated March 1, 2021.
</commit_message>
<xml_diff>
--- a/wrangle/data/interventions/place-types-concordance.xlsx
+++ b/wrangle/data/interventions/place-types-concordance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/CovidTimeline/wrangle/data/interventions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBE6208-0974-6542-8FE9-D7DF418840CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435C51F4-1ECB-0F44-9D52-AC228134D44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25960" windowHeight="11320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25960" windowHeight="11320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAICS" sheetId="1" r:id="rId1"/>
@@ -437,9 +437,6 @@
     <t>Estrie</t>
   </si>
   <si>
-    <t>simcoe muskoka, simoe, muskoka</t>
-  </si>
-  <si>
     <t>Simcoe Muskoka</t>
   </si>
   <si>
@@ -560,9 +557,6 @@
     <t>terms</t>
   </si>
   <si>
-    <t>health_reg</t>
-  </si>
-  <si>
     <t>personal care, non-essential services, salons, saunas, hair, wellness services</t>
   </si>
   <si>
@@ -651,15 +645,28 @@
   </si>
   <si>
     <t>Alcoholic Beverages</t>
+  </si>
+  <si>
+    <t>simcoe muskoka, simcoe, muskoka</t>
+  </si>
+  <si>
+    <t>Health Region</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -707,10 +714,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -718,9 +725,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2515,7 +2523,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2523,7 +2531,7 @@
         <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2531,7 +2539,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2539,7 +2547,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2547,7 +2555,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2555,7 +2563,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2571,7 +2579,7 @@
         <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2579,7 +2587,7 @@
         <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2591,8 +2599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F03E3E-5BAF-D645-88AF-65E5BAEFB672}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2603,51 +2611,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
-        <v>173</v>
+      <c r="A1" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2660,122 +2668,122 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B22" s="3" t="s">
         <v>132</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2859,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A589B64-3508-C44C-B4D4-EFDF33F16175}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
@@ -2875,10 +2883,10 @@
         <v>105</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2886,7 +2894,7 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2">
         <v>276</v>
@@ -2897,7 +2905,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>44</v>
@@ -2908,7 +2916,7 @@
         <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C4">
         <v>45</v>
@@ -2919,7 +2927,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5">
         <v>44</v>
@@ -2930,7 +2938,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6">
         <v>188</v>
@@ -2941,7 +2949,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -2952,7 +2960,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8">
         <v>121</v>
@@ -2963,7 +2971,7 @@
         <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C9">
         <v>277</v>
@@ -2974,7 +2982,7 @@
         <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C10">
         <v>68</v>
@@ -2985,7 +2993,7 @@
         <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2993,7 +3001,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C12">
         <v>60</v>
@@ -3001,7 +3009,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C13">
         <v>551</v>
@@ -3009,7 +3017,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -3017,7 +3025,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15">
         <v>423</v>
@@ -3025,7 +3033,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16">
         <v>1272</v>
@@ -3033,7 +3041,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17">
         <v>508</v>
@@ -3041,7 +3049,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18">
         <v>784</v>
@@ -3049,7 +3057,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C19">
         <v>1166</v>
@@ -3057,7 +3065,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20">
         <v>520</v>
@@ -3065,7 +3073,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C21">
         <v>29</v>
@@ -3073,7 +3081,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C22">
         <v>65</v>

</xml_diff>